<commit_message>
Last changes 2to 4164 100-150 timings until I get my hands on a few more example chips.
</commit_message>
<xml_diff>
--- a/firmware/timings/4164-120.xlsx
+++ b/firmware/timings/4164-120.xlsx
@@ -5294,7 +5294,7 @@
       </c>
       <c r="K5" s="28">
         <f>J5+(OFFSET($B$4,$I5,0)+1)*cmd_time</f>
-        <v>73.3326</v>
+        <v>69.9993</v>
       </c>
       <c r="L5" s="26" t="s">
         <v>20</v>
@@ -5305,7 +5305,7 @@
         <v>2.0</v>
       </c>
       <c r="B6" s="30">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -5320,11 +5320,11 @@
       </c>
       <c r="J6" s="27">
         <f t="shared" si="1"/>
-        <v>73.3326</v>
+        <v>69.9993</v>
       </c>
       <c r="K6" s="28">
         <f>J6+(OFFSET($B$4,$I6,0)+1)*cmd_time</f>
-        <v>76.6659</v>
+        <v>73.3326</v>
       </c>
       <c r="L6" s="26" t="s">
         <v>22</v>
@@ -5335,7 +5335,7 @@
         <v>3.0</v>
       </c>
       <c r="B7" s="30">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -5350,11 +5350,11 @@
       </c>
       <c r="J7" s="27">
         <f t="shared" si="1"/>
-        <v>76.6659</v>
+        <v>73.3326</v>
       </c>
       <c r="K7" s="28">
         <f>J7+(OFFSET($B$4,$I7,0)+1)*cmd_time</f>
-        <v>79.9992</v>
+        <v>76.6659</v>
       </c>
       <c r="L7" s="26" t="s">
         <v>24</v>
@@ -5380,11 +5380,11 @@
       </c>
       <c r="J8" s="27">
         <f t="shared" si="1"/>
-        <v>79.9992</v>
+        <v>76.6659</v>
       </c>
       <c r="K8" s="28">
         <f>J8+(OFFSET($B$4,$I8,0)+1)*cmd_time</f>
-        <v>96.6657</v>
+        <v>89.9991</v>
       </c>
       <c r="L8" s="26" t="s">
         <v>26</v>
@@ -5412,11 +5412,11 @@
       </c>
       <c r="J9" s="27">
         <f t="shared" si="1"/>
-        <v>96.6657</v>
+        <v>89.9991</v>
       </c>
       <c r="K9" s="28">
         <f>J9+(OFFSET($B$4,$I9,0)+1)*cmd_time</f>
-        <v>99.999</v>
+        <v>93.3324</v>
       </c>
       <c r="L9" s="26" t="s">
         <v>29</v>
@@ -5442,11 +5442,11 @@
       </c>
       <c r="J10" s="27">
         <f t="shared" si="1"/>
-        <v>99.999</v>
+        <v>93.3324</v>
       </c>
       <c r="K10" s="28">
         <f>J10+(OFFSET($B$4,$I10,0)+1)*cmd_time</f>
-        <v>103.3323</v>
+        <v>96.6657</v>
       </c>
       <c r="L10" s="26" t="s">
         <v>31</v>
@@ -5472,11 +5472,11 @@
       </c>
       <c r="J11" s="31">
         <f t="shared" si="1"/>
-        <v>103.3323</v>
+        <v>96.6657</v>
       </c>
       <c r="K11" s="28">
         <f>J11+(OFFSET($B$4,$I11,0)+1)*cmd_time</f>
-        <v>106.6656</v>
+        <v>99.999</v>
       </c>
       <c r="L11" s="26" t="s">
         <v>33</v>
@@ -5500,11 +5500,11 @@
       </c>
       <c r="J12" s="27">
         <f t="shared" si="1"/>
-        <v>106.6656</v>
+        <v>99.999</v>
       </c>
       <c r="K12" s="28">
         <f>J12+(OFFSET($B$4,$I12,0)+1)*cmd_time</f>
-        <v>109.9989</v>
+        <v>103.3323</v>
       </c>
       <c r="L12" s="26" t="s">
         <v>35</v>
@@ -5534,11 +5534,11 @@
       </c>
       <c r="J13" s="33">
         <f>K10</f>
-        <v>103.3323</v>
+        <v>96.6657</v>
       </c>
       <c r="K13" s="28">
         <f>J13+(OFFSET($B$4,$I13,0)+1)*cmd_time</f>
-        <v>106.6656</v>
+        <v>99.999</v>
       </c>
       <c r="L13" s="26" t="s">
         <v>41</v>
@@ -5557,7 +5557,7 @@
       </c>
       <c r="D14" s="35">
         <f>ROUND(ras_low_start - ras_high_end,1)</f>
-        <v>73.3</v>
+        <v>70</v>
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
@@ -5570,11 +5570,11 @@
       </c>
       <c r="J14" s="36">
         <f>K13</f>
-        <v>106.6656</v>
+        <v>99.999</v>
       </c>
       <c r="K14" s="28">
         <f>J14+(OFFSET($B$4,$I14,0)+1)*cmd_time</f>
-        <v>109.9989</v>
+        <v>103.3323</v>
       </c>
       <c r="L14" s="26" t="s">
         <v>44</v>
@@ -5593,7 +5593,7 @@
       </c>
       <c r="D15" s="35">
         <f>ROUND(asc_start - ras_low_end, 1)</f>
-        <v>16.7</v>
+        <v>13.3</v>
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
@@ -5608,11 +5608,11 @@
       </c>
       <c r="J15" s="27">
         <f>K12</f>
-        <v>109.9989</v>
+        <v>103.3323</v>
       </c>
       <c r="K15" s="28">
         <f>J15+(OFFSET($B$4,$I15,0)+1)*cmd_time</f>
-        <v>113.3322</v>
+        <v>106.6656</v>
       </c>
       <c r="L15" s="26" t="s">
         <v>48</v>
@@ -5631,7 +5631,7 @@
       </c>
       <c r="D16" s="35">
         <f>ROUND(max(cas_low_start_w-cas_high_end,cas_low_start_r-cas_high_end),1)</f>
-        <v>100</v>
+        <v>93.3</v>
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
@@ -5644,11 +5644,11 @@
       </c>
       <c r="J16" s="27">
         <f t="shared" ref="J16:J24" si="2">K15</f>
-        <v>113.3322</v>
+        <v>106.6656</v>
       </c>
       <c r="K16" s="28">
         <f>J16+(OFFSET($B$4,$I16,0)+1)*cmd_time</f>
-        <v>166.665</v>
+        <v>159.9984</v>
       </c>
       <c r="L16" s="26" t="s">
         <v>51</v>
@@ -5667,7 +5667,7 @@
       </c>
       <c r="D17" s="35">
         <f>ROUND(cas_low_start_w - ras_low_end,1)</f>
-        <v>23.3</v>
+        <v>20</v>
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="20"/>
@@ -5680,11 +5680,11 @@
       </c>
       <c r="J17" s="27">
         <f t="shared" si="2"/>
-        <v>166.665</v>
+        <v>159.9984</v>
       </c>
       <c r="K17" s="28">
         <f>J17+(OFFSET($B$4,$I17,0)+1)*cmd_time</f>
-        <v>169.9983</v>
+        <v>163.3317</v>
       </c>
       <c r="L17" s="26" t="s">
         <v>53</v>
@@ -5703,7 +5703,7 @@
       </c>
       <c r="D18" s="35">
         <f>ROUND(cas_low_start_w - ras_low_end,1)</f>
-        <v>23.3</v>
+        <v>20</v>
       </c>
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
@@ -5716,11 +5716,11 @@
       </c>
       <c r="J18" s="27">
         <f t="shared" si="2"/>
-        <v>169.9983</v>
+        <v>163.3317</v>
       </c>
       <c r="K18" s="28">
         <f>J18+(OFFSET($B$4,$I18,0)+1)*cmd_time</f>
-        <v>173.3316</v>
+        <v>166.665</v>
       </c>
       <c r="L18" s="37" t="s">
         <v>55</v>
@@ -5752,11 +5752,11 @@
       </c>
       <c r="J19" s="27">
         <f t="shared" si="2"/>
-        <v>173.3316</v>
+        <v>166.665</v>
       </c>
       <c r="K19" s="28">
         <f>J19+(OFFSET($B$4,$I19,0)+1)*cmd_time</f>
-        <v>189.9981</v>
+        <v>183.3315</v>
       </c>
       <c r="L19" s="26" t="s">
         <v>58</v>
@@ -5788,11 +5788,11 @@
       </c>
       <c r="J20" s="27">
         <f t="shared" si="2"/>
-        <v>189.9981</v>
+        <v>183.3315</v>
       </c>
       <c r="K20" s="28">
         <f>J20+(OFFSET($B$4,$I20,0)+1)*cmd_time</f>
-        <v>193.3314</v>
+        <v>186.6648</v>
       </c>
       <c r="L20" s="26" t="s">
         <v>61</v>
@@ -5811,7 +5811,7 @@
       </c>
       <c r="D21" s="35">
         <f>ROUND(w_high_start_2 - ras_low_end, 1)</f>
-        <v>86.7</v>
+        <v>83.3</v>
       </c>
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
@@ -5824,11 +5824,11 @@
       </c>
       <c r="J21" s="27">
         <f t="shared" si="2"/>
-        <v>193.3314</v>
+        <v>186.6648</v>
       </c>
       <c r="K21" s="28">
         <f>J21+(OFFSET($B$4,$I21,0)+1)*cmd_time</f>
-        <v>196.6647</v>
+        <v>189.9981</v>
       </c>
       <c r="L21" s="26" t="s">
         <v>63</v>
@@ -5860,11 +5860,11 @@
       </c>
       <c r="J22" s="27">
         <f t="shared" si="2"/>
-        <v>196.6647</v>
+        <v>189.9981</v>
       </c>
       <c r="K22" s="28">
         <f>J22+(OFFSET($B$4,$I22,0)+1)*cmd_time</f>
-        <v>199.998</v>
+        <v>193.3314</v>
       </c>
       <c r="L22" s="26"/>
     </row>
@@ -5881,7 +5881,7 @@
       </c>
       <c r="D23" s="39">
         <f>round(d_clear_start - ras_low_end, 1)</f>
-        <v>90</v>
+        <v>86.7</v>
       </c>
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>
@@ -5894,11 +5894,11 @@
       </c>
       <c r="J23" s="27">
         <f t="shared" si="2"/>
-        <v>199.998</v>
+        <v>193.3314</v>
       </c>
       <c r="K23" s="28">
         <f>J23+(OFFSET($B$4,$I23,0)+1)*cmd_time</f>
-        <v>203.3313</v>
+        <v>196.6647</v>
       </c>
       <c r="L23" s="26" t="s">
         <v>68</v>
@@ -5917,7 +5917,7 @@
       </c>
       <c r="D24" s="35">
         <f>ROUND(valid_data_start -ras_low_end, 1)</f>
-        <v>110</v>
+        <v>106.7</v>
       </c>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
@@ -5930,11 +5930,11 @@
       </c>
       <c r="J24" s="27">
         <f t="shared" si="2"/>
-        <v>203.3313</v>
+        <v>196.6647</v>
       </c>
       <c r="K24" s="28">
         <f>J24+(OFFSET($B$4,$I24,0)+1)*cmd_time</f>
-        <v>206.6646</v>
+        <v>199.998</v>
       </c>
       <c r="L24" s="40" t="s">
         <v>71</v>
@@ -5986,7 +5986,7 @@
       </c>
       <c r="D26" s="35">
         <f>ROUND(cas_high_start - ras_low_end,1)</f>
-        <v>113.3</v>
+        <v>110</v>
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
@@ -6059,7 +6059,7 @@
       </c>
       <c r="D28" s="35">
         <f>ROUND(ras_high_start - ras_low_end, 1)</f>
-        <v>126.7</v>
+        <v>123.3</v>
       </c>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
@@ -6093,7 +6093,7 @@
       </c>
       <c r="D29" s="35">
         <f>ras_high_start</f>
-        <v>206.6646</v>
+        <v>199.998</v>
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>

</xml_diff>